<commit_message>
add more ATS estimates to the time series
</commit_message>
<xml_diff>
--- a/1. data/Barkley-Sk_pre-smolt_abundances.xlsx
+++ b/1. data/Barkley-Sk_pre-smolt_abundances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055FBC1F-361D-402F-A563-A6E69B7F02CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB19D0AE-3FF2-4634-9D94-E12E568BC19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93B9BABA-C468-4873-970E-7D7E9A90394F}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ATS_estimates!$A$1:$I$96</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -610,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CDFEE8-69FE-4C98-AD8C-E5081C486B0D}">
   <dimension ref="A1:J307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A295" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E271" sqref="E271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7423,7 +7423,7 @@
         <v>41716</v>
       </c>
       <c r="D206" s="4">
-        <f t="shared" si="21"/>
+        <f>IF(MONTH(C206)&lt;4,B206-2,B206-1)</f>
         <v>2012</v>
       </c>
       <c r="E206" s="4">
@@ -9588,16 +9588,13 @@
         <v>12</v>
       </c>
       <c r="B271">
-        <f t="shared" si="25"/>
-        <v>1900</v>
+        <v>2002</v>
       </c>
       <c r="D271" s="4">
-        <f t="shared" si="28"/>
-        <v>1898</v>
+        <v>2001</v>
       </c>
       <c r="E271" s="4">
-        <f t="shared" si="29"/>
-        <v>1897</v>
+        <v>2000</v>
       </c>
       <c r="G271" s="9"/>
     </row>
@@ -10850,7 +10847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E33CA0F3-68C3-4F60-B516-F4CB80D1245F}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add Nov 1979 infilled estimate for Hucuktlis
</commit_message>
<xml_diff>
--- a/1. data/Barkley-Sk_pre-smolt_abundances.xlsx
+++ b/1. data/Barkley-Sk_pre-smolt_abundances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB19D0AE-3FF2-4634-9D94-E12E568BC19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE94DA91-C754-4CC7-852D-8C06ACF18513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93B9BABA-C468-4873-970E-7D7E9A90394F}"/>
   </bookViews>
@@ -44,6 +44,8 @@
   <authors>
     <author>tc={51828A2D-7DC2-4829-B811-13295E6A575B}</author>
     <author>Brown, Nicholas</author>
+    <author>tc={9450F348-AFEB-4317-AD43-51976EFBA421}</author>
+    <author>tc={C335BF2D-8A76-4A85-B639-EC939DD5E53A}</author>
   </authors>
   <commentList>
     <comment ref="G1" authorId="0" shapeId="0" xr:uid="{51828A2D-7DC2-4829-B811-13295E6A575B}">
@@ -100,6 +102,22 @@
           <t xml:space="preserve">
 My choice, overriding Hyatt's choice.</t>
         </r>
+      </text>
+    </comment>
+    <comment ref="F112" authorId="2" shapeId="0" xr:uid="{9450F348-AFEB-4317-AD43-51976EFBA421}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    From Howard Stiff via log-linear regression of total abundance versus smolt length (62mm in Nov 1979) in Hucuktlis Lake.</t>
+      </text>
+    </comment>
+    <comment ref="G112" authorId="3" shapeId="0" xr:uid="{C335BF2D-8A76-4A85-B639-EC939DD5E53A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1977-1985 average CV applied to guesstimated mean</t>
       </text>
     </comment>
     <comment ref="J251" authorId="1" shapeId="0" xr:uid="{F52DD24B-5ABC-4F49-A632-F9389FACE903}">
@@ -204,7 +222,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +258,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -279,6 +304,8 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -603,6 +630,12 @@
   <threadedComment ref="G1" dT="2025-02-07T20:07:08.24" personId="{3DE5C77A-2EC9-410D-AF92-25A6BD2452F6}" id="{51828A2D-7DC2-4829-B811-13295E6A575B}">
     <text xml:space="preserve">SD? =sqrt(sum(transect variances)/N transects) </text>
   </threadedComment>
+  <threadedComment ref="F112" dT="2025-03-04T16:49:42.59" personId="{3DE5C77A-2EC9-410D-AF92-25A6BD2452F6}" id="{9450F348-AFEB-4317-AD43-51976EFBA421}">
+    <text>From Howard Stiff via log-linear regression of total abundance versus smolt length (62mm in Nov 1979) in Hucuktlis Lake.</text>
+  </threadedComment>
+  <threadedComment ref="G112" dT="2025-03-04T16:50:12.85" personId="{3DE5C77A-2EC9-410D-AF92-25A6BD2452F6}" id="{C335BF2D-8A76-4A85-B639-EC939DD5E53A}">
+    <text>1977-1985 average CV applied to guesstimated mean</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -610,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CDFEE8-69FE-4C98-AD8C-E5081C486B0D}">
   <dimension ref="A1:J307"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E271" sqref="E271"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4261,6 +4294,13 @@
       <c r="E112" s="4">
         <f t="shared" si="10"/>
         <v>1977</v>
+      </c>
+      <c r="F112" s="10">
+        <v>1000000</v>
+      </c>
+      <c r="G112" s="11">
+        <f>(SUM(G109:G111,G113:G128)/SUM(F109:F111,F113:F128))*F112</f>
+        <v>363579.76303034025</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update estimated 1979 Hucuktlis fry estimate
</commit_message>
<xml_diff>
--- a/1. data/Barkley-Sk_pre-smolt_abundances.xlsx
+++ b/1. data/Barkley-Sk_pre-smolt_abundances.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brownn\Documents\WCVI\Barkley-Sk-CSAS\1. data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE94DA91-C754-4CC7-852D-8C06ACF18513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC51F338-AF2D-4FB0-BC0A-317A9970497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{93B9BABA-C468-4873-970E-7D7E9A90394F}"/>
   </bookViews>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CDFEE8-69FE-4C98-AD8C-E5081C486B0D}">
   <dimension ref="A1:J307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="H112" sqref="H112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4301,6 +4301,9 @@
       <c r="G112" s="11">
         <f>(SUM(G109:G111,G113:G128)/SUM(F109:F111,F113:F128))*F112</f>
         <v>363579.76303034025</v>
+      </c>
+      <c r="J112">
+        <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>